<commit_message>
changed to a simpler test
</commit_message>
<xml_diff>
--- a/tests/xlsx/date.xlsx
+++ b/tests/xlsx/date.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27226"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA3ABC04-0246-4D85-BA10-9892E4EBD8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6284DFCA-3C56-4D46-8321-3FF7F1659C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,10 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="177" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="178" formatCode="[$-409]mmm\-yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -66,12 +65,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -389,28 +386,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>45287</v>
+        <v>44928</v>
       </c>
       <c r="B1" s="2">
-        <v>45288</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3">
-        <v>45286</v>
+      <c r="A2" s="1">
+        <v>44929</v>
       </c>
-      <c r="B2" s="4">
-        <v>45285</v>
+      <c r="B2" s="2">
+        <v>44929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the test file
</commit_message>
<xml_diff>
--- a/tests/xlsx/date.xlsx
+++ b/tests/xlsx/date.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6284DFCA-3C56-4D46-8321-3FF7F1659C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0BB167D-F30E-4AB7-B915-91DABD4115DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,31 +383,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1">
-        <v>44928</v>
-      </c>
-      <c r="B1" s="2">
-        <v>44928</v>
+        <v>45306</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>44929</v>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2">
+        <v>45306</v>
       </c>
-      <c r="B2" s="2">
-        <v>44929</v>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1">
+        <v>45306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>